<commit_message>
Week 16.9 - Enforcing a One-to-Many Relationship
</commit_message>
<xml_diff>
--- a/Week16/Excel database example.xlsx
+++ b/Week16/Excel database example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\SourceCode\JavaBootcamp\Week16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E95ABBC2-B731-4029-882E-45A4CFCC43BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4702E2DB-AC7D-460A-93E5-16C6B1982058}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34425" yWindow="6930" windowWidth="28800" windowHeight="15435" xr2:uid="{FF5F90E8-EBBF-42ED-A91E-4779DC26B041}"/>
+    <workbookView xWindow="-19005" yWindow="5910" windowWidth="28800" windowHeight="15435" xr2:uid="{FF5F90E8-EBBF-42ED-A91E-4779DC26B041}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>